<commit_message>
latest % mature fig and stats; AD main figure
</commit_message>
<xml_diff>
--- a/FishLandings/household groups/statistics/Biomass (kg)_output.xlsx
+++ b/FishLandings/household groups/statistics/Biomass (kg)_output.xlsx
@@ -416,13 +416,13 @@
         </is>
       </c>
       <c r="B2">
-        <v>569.062204</v>
+        <v>823.1006599999999</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2">
-        <v>54.631182</v>
+        <v>92.893722</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -440,16 +440,16 @@
         </is>
       </c>
       <c r="B3">
-        <v>144.664285</v>
+        <v>259.839611</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3">
-        <v>6.94404</v>
+        <v>14.662525</v>
       </c>
       <c r="E3">
-        <v>0.001187</v>
+        <v>1e-06</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -464,10 +464,10 @@
         </is>
       </c>
       <c r="B4">
-        <v>2322.86518</v>
+        <v>2941.742588</v>
       </c>
       <c r="C4">
-        <v>223</v>
+        <v>332</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -487,16 +487,16 @@
         </is>
       </c>
       <c r="G5">
-        <v>-1.286</v>
+        <v>-1.439321</v>
       </c>
       <c r="H5">
-        <v>-2.695544</v>
+        <v>-2.518559</v>
       </c>
       <c r="I5">
-        <v>0.123544</v>
+        <v>-0.360083</v>
       </c>
       <c r="J5">
-        <v>0.081815</v>
+        <v>0.005224</v>
       </c>
     </row>
     <row r="6">
@@ -511,16 +511,16 @@
         </is>
       </c>
       <c r="G6">
-        <v>0.444548</v>
+        <v>0.443477</v>
       </c>
       <c r="H6">
-        <v>-1.073233</v>
+        <v>-0.690089</v>
       </c>
       <c r="I6">
-        <v>1.962329</v>
+        <v>1.577043</v>
       </c>
       <c r="J6">
-        <v>0.76895</v>
+        <v>0.62737</v>
       </c>
     </row>
     <row r="7">
@@ -535,16 +535,16 @@
         </is>
       </c>
       <c r="G7">
-        <v>1.730548</v>
+        <v>1.882798</v>
       </c>
       <c r="H7">
-        <v>0.58309</v>
+        <v>1.030432</v>
       </c>
       <c r="I7">
-        <v>2.878006</v>
+        <v>2.735164</v>
       </c>
       <c r="J7">
-        <v>0.00132</v>
+        <v>1e-06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>